<commit_message>
Removed extra axis printing in MP4 plots
</commit_message>
<xml_diff>
--- a/www/MP4/NGA_summary.xlsx
+++ b/www/MP4/NGA_summary.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X11"/>
+  <dimension ref="A1:X6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -482,7 +482,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021-09-01</t>
+          <t>2020-09-01</t>
         </is>
       </c>
       <c r="B2">
@@ -507,7 +507,7 @@
         <v>2469</v>
       </c>
       <c r="I2">
-        <v>20428.07498118222</v>
+        <v>0</v>
       </c>
       <c r="J2">
         <v>20.12069824546279</v>
@@ -528,7 +528,7 @@
         <v>11206</v>
       </c>
       <c r="P2">
-        <v>0.0001</v>
+        <v>0</v>
       </c>
       <c r="Q2">
         <v>0.0001</v>
@@ -550,7 +550,7 @@
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>SVEIRD</t>
+          <t>SEIRD</t>
         </is>
       </c>
       <c r="X2">
@@ -560,17 +560,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021-09-02</t>
+          <t>2020-09-02</t>
         </is>
       </c>
       <c r="B3">
         <v>206527214</v>
       </c>
       <c r="C3">
-        <v>204260302</v>
+        <v>204280730</v>
       </c>
       <c r="D3">
-        <v>2018428</v>
+        <v>1998000</v>
       </c>
       <c r="E3">
         <v>55602</v>
@@ -585,7 +585,7 @@
         <v>2480</v>
       </c>
       <c r="I3">
-        <v>20428.07498118222</v>
+        <v>0</v>
       </c>
       <c r="J3">
         <v>19.59756009108077</v>
@@ -606,7 +606,7 @@
         <v>11654</v>
       </c>
       <c r="P3">
-        <v>0.0001</v>
+        <v>0</v>
       </c>
       <c r="Q3">
         <v>0.0001</v>
@@ -628,7 +628,7 @@
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>SVEIRD</t>
+          <t>SEIRD</t>
         </is>
       </c>
       <c r="X3">
@@ -638,17 +638,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021-09-03</t>
+          <t>2020-09-03</t>
         </is>
       </c>
       <c r="B4">
         <v>206527214</v>
       </c>
       <c r="C4">
-        <v>204260302</v>
+        <v>204280730</v>
       </c>
       <c r="D4">
-        <v>2018428</v>
+        <v>1998000</v>
       </c>
       <c r="E4">
         <v>55601</v>
@@ -663,7 +663,7 @@
         <v>2491</v>
       </c>
       <c r="I4">
-        <v>20428.07498118222</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <v>19.59756009108077</v>
@@ -684,7 +684,7 @@
         <v>12102</v>
       </c>
       <c r="P4">
-        <v>0.0001</v>
+        <v>0</v>
       </c>
       <c r="Q4">
         <v>0.0001</v>
@@ -706,7 +706,7 @@
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>SVEIRD</t>
+          <t>SEIRD</t>
         </is>
       </c>
       <c r="X4">
@@ -716,17 +716,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021-09-04</t>
+          <t>2020-09-04</t>
         </is>
       </c>
       <c r="B5">
         <v>206527214</v>
       </c>
       <c r="C5">
-        <v>204260302</v>
+        <v>204280730</v>
       </c>
       <c r="D5">
-        <v>2018428</v>
+        <v>1998000</v>
       </c>
       <c r="E5">
         <v>55601</v>
@@ -741,7 +741,7 @@
         <v>2503</v>
       </c>
       <c r="I5">
-        <v>20428.07498118222</v>
+        <v>0</v>
       </c>
       <c r="J5">
         <v>19.59756009108077</v>
@@ -762,7 +762,7 @@
         <v>12551</v>
       </c>
       <c r="P5">
-        <v>0.0001</v>
+        <v>0</v>
       </c>
       <c r="Q5">
         <v>0.0001</v>
@@ -784,7 +784,7 @@
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>SVEIRD</t>
+          <t>SEIRD</t>
         </is>
       </c>
       <c r="X5">
@@ -794,17 +794,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021-09-05</t>
+          <t>2020-09-05</t>
         </is>
       </c>
       <c r="B6">
         <v>206527214</v>
       </c>
       <c r="C6">
-        <v>204260302</v>
+        <v>204280730</v>
       </c>
       <c r="D6">
-        <v>2018428</v>
+        <v>1998000</v>
       </c>
       <c r="E6">
         <v>55601</v>
@@ -819,7 +819,7 @@
         <v>2514</v>
       </c>
       <c r="I6">
-        <v>20428.07498118222</v>
+        <v>0</v>
       </c>
       <c r="J6">
         <v>19.59756009108077</v>
@@ -840,7 +840,7 @@
         <v>12999</v>
       </c>
       <c r="P6">
-        <v>0.0001</v>
+        <v>0</v>
       </c>
       <c r="Q6">
         <v>0.0001</v>
@@ -862,400 +862,10 @@
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>SVEIRD</t>
+          <t>SEIRD</t>
         </is>
       </c>
       <c r="X6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2021-09-06</t>
-        </is>
-      </c>
-      <c r="B7">
-        <v>206527214</v>
-      </c>
-      <c r="C7">
-        <v>204260302</v>
-      </c>
-      <c r="D7">
-        <v>2018428</v>
-      </c>
-      <c r="E7">
-        <v>55601</v>
-      </c>
-      <c r="F7">
-        <v>10915</v>
-      </c>
-      <c r="G7">
-        <v>182401</v>
-      </c>
-      <c r="H7">
-        <v>2525</v>
-      </c>
-      <c r="I7">
-        <v>20428.07498118222</v>
-      </c>
-      <c r="J7">
-        <v>19.59756009108077</v>
-      </c>
-      <c r="K7">
-        <v>448.2399999999999</v>
-      </c>
-      <c r="L7">
-        <v>728.3900000000001</v>
-      </c>
-      <c r="M7">
-        <v>11.206</v>
-      </c>
-      <c r="N7">
-        <v>56129</v>
-      </c>
-      <c r="O7">
-        <v>13447</v>
-      </c>
-      <c r="P7">
-        <v>0.0001</v>
-      </c>
-      <c r="Q7">
-        <v>0.0001</v>
-      </c>
-      <c r="R7">
-        <v>0.008</v>
-      </c>
-      <c r="S7">
-        <v>0.065</v>
-      </c>
-      <c r="T7">
-        <v>0.001</v>
-      </c>
-      <c r="U7">
-        <v>2</v>
-      </c>
-      <c r="V7">
-        <v>25</v>
-      </c>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>SVEIRD</t>
-        </is>
-      </c>
-      <c r="X7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2021-09-07</t>
-        </is>
-      </c>
-      <c r="B8">
-        <v>206527214</v>
-      </c>
-      <c r="C8">
-        <v>204260302</v>
-      </c>
-      <c r="D8">
-        <v>2018428</v>
-      </c>
-      <c r="E8">
-        <v>55601</v>
-      </c>
-      <c r="F8">
-        <v>10915</v>
-      </c>
-      <c r="G8">
-        <v>183129</v>
-      </c>
-      <c r="H8">
-        <v>2536</v>
-      </c>
-      <c r="I8">
-        <v>20428.07498118222</v>
-      </c>
-      <c r="J8">
-        <v>19.59756009108077</v>
-      </c>
-      <c r="K8">
-        <v>448.2399999999999</v>
-      </c>
-      <c r="L8">
-        <v>728.3900000000001</v>
-      </c>
-      <c r="M8">
-        <v>11.206</v>
-      </c>
-      <c r="N8">
-        <v>56148</v>
-      </c>
-      <c r="O8">
-        <v>13895</v>
-      </c>
-      <c r="P8">
-        <v>0.0001</v>
-      </c>
-      <c r="Q8">
-        <v>0.0001</v>
-      </c>
-      <c r="R8">
-        <v>0.008</v>
-      </c>
-      <c r="S8">
-        <v>0.065</v>
-      </c>
-      <c r="T8">
-        <v>0.001</v>
-      </c>
-      <c r="U8">
-        <v>2</v>
-      </c>
-      <c r="V8">
-        <v>25</v>
-      </c>
-      <c r="W8" t="inlineStr">
-        <is>
-          <t>SVEIRD</t>
-        </is>
-      </c>
-      <c r="X8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2021-09-08</t>
-        </is>
-      </c>
-      <c r="B9">
-        <v>206527214</v>
-      </c>
-      <c r="C9">
-        <v>204260302</v>
-      </c>
-      <c r="D9">
-        <v>2018428</v>
-      </c>
-      <c r="E9">
-        <v>55601</v>
-      </c>
-      <c r="F9">
-        <v>10915</v>
-      </c>
-      <c r="G9">
-        <v>183858</v>
-      </c>
-      <c r="H9">
-        <v>2547</v>
-      </c>
-      <c r="I9">
-        <v>20428.07498118222</v>
-      </c>
-      <c r="J9">
-        <v>19.59756009108077</v>
-      </c>
-      <c r="K9">
-        <v>448.2399999999999</v>
-      </c>
-      <c r="L9">
-        <v>728.3900000000001</v>
-      </c>
-      <c r="M9">
-        <v>11.206</v>
-      </c>
-      <c r="N9">
-        <v>56168</v>
-      </c>
-      <c r="O9">
-        <v>14344</v>
-      </c>
-      <c r="P9">
-        <v>0.0001</v>
-      </c>
-      <c r="Q9">
-        <v>0.0001</v>
-      </c>
-      <c r="R9">
-        <v>0.008</v>
-      </c>
-      <c r="S9">
-        <v>0.065</v>
-      </c>
-      <c r="T9">
-        <v>0.001</v>
-      </c>
-      <c r="U9">
-        <v>2</v>
-      </c>
-      <c r="V9">
-        <v>25</v>
-      </c>
-      <c r="W9" t="inlineStr">
-        <is>
-          <t>SVEIRD</t>
-        </is>
-      </c>
-      <c r="X9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2021-09-09</t>
-        </is>
-      </c>
-      <c r="B10">
-        <v>206527214</v>
-      </c>
-      <c r="C10">
-        <v>204260302</v>
-      </c>
-      <c r="D10">
-        <v>2018428</v>
-      </c>
-      <c r="E10">
-        <v>55601</v>
-      </c>
-      <c r="F10">
-        <v>10915</v>
-      </c>
-      <c r="G10">
-        <v>184586</v>
-      </c>
-      <c r="H10">
-        <v>2559</v>
-      </c>
-      <c r="I10">
-        <v>20428.07498118222</v>
-      </c>
-      <c r="J10">
-        <v>19.59756009108077</v>
-      </c>
-      <c r="K10">
-        <v>448.2399999999999</v>
-      </c>
-      <c r="L10">
-        <v>728.3900000000001</v>
-      </c>
-      <c r="M10">
-        <v>11.206</v>
-      </c>
-      <c r="N10">
-        <v>56187</v>
-      </c>
-      <c r="O10">
-        <v>14792</v>
-      </c>
-      <c r="P10">
-        <v>0.0001</v>
-      </c>
-      <c r="Q10">
-        <v>0.0001</v>
-      </c>
-      <c r="R10">
-        <v>0.008</v>
-      </c>
-      <c r="S10">
-        <v>0.065</v>
-      </c>
-      <c r="T10">
-        <v>0.001</v>
-      </c>
-      <c r="U10">
-        <v>2</v>
-      </c>
-      <c r="V10">
-        <v>25</v>
-      </c>
-      <c r="W10" t="inlineStr">
-        <is>
-          <t>SVEIRD</t>
-        </is>
-      </c>
-      <c r="X10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2021-09-10</t>
-        </is>
-      </c>
-      <c r="B11">
-        <v>206527214</v>
-      </c>
-      <c r="C11">
-        <v>204260302</v>
-      </c>
-      <c r="D11">
-        <v>2018428</v>
-      </c>
-      <c r="E11">
-        <v>55601</v>
-      </c>
-      <c r="F11">
-        <v>10915</v>
-      </c>
-      <c r="G11">
-        <v>185315</v>
-      </c>
-      <c r="H11">
-        <v>2570</v>
-      </c>
-      <c r="I11">
-        <v>20428.07498118222</v>
-      </c>
-      <c r="J11">
-        <v>19.59756009108077</v>
-      </c>
-      <c r="K11">
-        <v>448.2399999999999</v>
-      </c>
-      <c r="L11">
-        <v>728.3900000000001</v>
-      </c>
-      <c r="M11">
-        <v>11.206</v>
-      </c>
-      <c r="N11">
-        <v>56207</v>
-      </c>
-      <c r="O11">
-        <v>15240</v>
-      </c>
-      <c r="P11">
-        <v>0.0001</v>
-      </c>
-      <c r="Q11">
-        <v>0.0001</v>
-      </c>
-      <c r="R11">
-        <v>0.008</v>
-      </c>
-      <c r="S11">
-        <v>0.065</v>
-      </c>
-      <c r="T11">
-        <v>0.001</v>
-      </c>
-      <c r="U11">
-        <v>2</v>
-      </c>
-      <c r="V11">
-        <v>25</v>
-      </c>
-      <c r="W11" t="inlineStr">
-        <is>
-          <t>SVEIRD</t>
-        </is>
-      </c>
-      <c r="X11">
         <v>0</v>
       </c>
     </row>

</xml_diff>